<commit_message>
Update video path in final1.py
</commit_message>
<xml_diff>
--- a/COCO Dataset Classes.xlsx
+++ b/COCO Dataset Classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/md.sazibahmed/Downloads/Thesis/Prototype_up/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12CFDE4-18A2-5448-AD9A-D384C823850F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08621906-8E2D-324B-A239-15A442A6A920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="29400" windowHeight="17180" xr2:uid="{E07CE1F7-7C86-9144-BB3F-DB4CF0B8220A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" xr2:uid="{E07CE1F7-7C86-9144-BB3F-DB4CF0B8220A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="191">
   <si>
     <t>ID</t>
   </si>
@@ -2526,10 +2526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FD8F19-BF0C-0D4A-959B-A1D4C7CC9A6C}">
-  <dimension ref="A2:H81"/>
+  <dimension ref="A2:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2539,14 +2539,16 @@
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="7" max="7" width="22.6640625" customWidth="1"/>
     <col min="8" max="8" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>109</v>
       </c>
@@ -2558,8 +2560,12 @@
         <v>189</v>
       </c>
       <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>110</v>
       </c>
@@ -2575,8 +2581,14 @@
       <c r="H4" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>188</v>
+      </c>
+      <c r="K4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>111</v>
       </c>
@@ -2592,8 +2604,14 @@
       <c r="H5" s="19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>112</v>
       </c>
@@ -2609,8 +2627,14 @@
       <c r="H6" s="19" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>113</v>
       </c>
@@ -2626,8 +2650,14 @@
       <c r="H7" s="19" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>114</v>
       </c>
@@ -2643,8 +2673,14 @@
       <c r="H8" s="19" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>115</v>
       </c>
@@ -2660,8 +2696,14 @@
       <c r="H9" s="19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>116</v>
       </c>
@@ -2677,8 +2719,14 @@
       <c r="H10" s="19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>117</v>
       </c>
@@ -2694,8 +2742,14 @@
       <c r="H11" s="19" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J11" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>118</v>
       </c>
@@ -2711,8 +2765,14 @@
       <c r="H12" s="19" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J12" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>119</v>
       </c>
@@ -2728,8 +2788,14 @@
       <c r="H13" s="19" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>120</v>
       </c>
@@ -2745,8 +2811,14 @@
       <c r="H14" s="16" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J14" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>121</v>
       </c>
@@ -2762,8 +2834,12 @@
       <c r="H15" s="16" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J15" s="19"/>
+      <c r="K15" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>122</v>
       </c>
@@ -2779,8 +2855,12 @@
       <c r="H16" s="19" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16" s="19"/>
+      <c r="K16" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>123</v>
       </c>
@@ -2796,8 +2876,11 @@
       <c r="H17" s="19" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K17" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>124</v>
       </c>
@@ -2807,8 +2890,11 @@
       <c r="H18" s="19" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K18" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>125</v>
       </c>
@@ -2818,8 +2904,11 @@
       <c r="H19" s="19" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K19" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>126</v>
       </c>
@@ -2829,8 +2918,11 @@
       <c r="H20" s="19" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K20" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>127</v>
       </c>
@@ -2840,8 +2932,11 @@
       <c r="H21" s="19" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K21" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>128</v>
       </c>
@@ -2851,8 +2946,11 @@
       <c r="H22" s="19" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K22" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>129</v>
       </c>
@@ -2862,8 +2960,11 @@
       <c r="H23" s="16" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K23" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>130</v>
       </c>
@@ -2873,8 +2974,11 @@
       <c r="H24" s="16" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K24" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>131</v>
       </c>
@@ -2884,8 +2988,11 @@
       <c r="H25" s="16" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K25" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>132</v>
       </c>
@@ -2895,8 +3002,11 @@
       <c r="H26" s="16" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K26" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>133</v>
       </c>
@@ -2906,8 +3016,11 @@
       <c r="H27" s="16" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K27" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>134</v>
       </c>
@@ -2917,8 +3030,11 @@
       <c r="H28" s="19" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K28" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>135</v>
       </c>
@@ -2928,8 +3044,11 @@
       <c r="H29" s="19" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K29" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>136</v>
       </c>
@@ -2939,8 +3058,11 @@
       <c r="H30" s="19" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K30" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>137</v>
       </c>
@@ -2951,7 +3073,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>138</v>
       </c>
@@ -2961,8 +3083,9 @@
       <c r="H32" s="19" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K32" s="19"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>139</v>
       </c>
@@ -2972,8 +3095,9 @@
       <c r="H33" s="19" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>140</v>
       </c>
@@ -2983,8 +3107,9 @@
       <c r="H34" s="19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K34" s="19"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>141</v>
       </c>
@@ -2994,8 +3119,9 @@
       <c r="H35" s="19" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K35" s="19"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>142</v>
       </c>
@@ -3005,8 +3131,9 @@
       <c r="H36" s="19" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K36" s="19"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>143</v>
       </c>
@@ -3016,8 +3143,9 @@
       <c r="H37" s="19" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K37" s="19"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>144</v>
       </c>
@@ -3028,7 +3156,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>145</v>
       </c>
@@ -3038,8 +3166,9 @@
       <c r="H39" s="19" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>146</v>
       </c>
@@ -3050,7 +3179,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>147</v>
       </c>
@@ -3061,7 +3190,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>148</v>
       </c>
@@ -3072,7 +3201,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>149</v>
       </c>
@@ -3083,7 +3212,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>150</v>
       </c>
@@ -3094,7 +3223,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>151</v>
       </c>
@@ -3104,8 +3233,9 @@
       <c r="H45" s="19" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K45" s="19"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>152</v>
       </c>
@@ -3115,8 +3245,9 @@
       <c r="H46" s="19" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K46" s="19"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>153</v>
       </c>
@@ -3126,8 +3257,9 @@
       <c r="H47" s="19" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K47" s="19"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
         <v>154</v>
       </c>
@@ -3137,8 +3269,9 @@
       <c r="H48" s="19" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K48" s="19"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
         <v>155</v>
       </c>
@@ -3148,8 +3281,9 @@
       <c r="H49" s="19" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K49" s="19"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
         <v>156</v>
       </c>
@@ -3159,8 +3293,9 @@
       <c r="H50" s="19" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K50" s="19"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="s">
         <v>157</v>
       </c>
@@ -3170,8 +3305,9 @@
       <c r="H51" s="19" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K51" s="19"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="s">
         <v>158</v>
       </c>
@@ -3181,8 +3317,9 @@
       <c r="H52" s="19" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K52" s="19"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
         <v>159</v>
       </c>
@@ -3192,8 +3329,9 @@
       <c r="H53" s="19" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K53" s="19"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
         <v>160</v>
       </c>
@@ -3203,8 +3341,9 @@
       <c r="H54" s="19" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K54" s="19"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="16" t="s">
         <v>161</v>
       </c>
@@ -3215,7 +3354,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
         <v>162</v>
       </c>
@@ -3226,7 +3365,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="16" t="s">
         <v>163</v>
       </c>
@@ -3237,7 +3376,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>164</v>
       </c>
@@ -3248,7 +3387,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>165</v>
       </c>
@@ -3259,7 +3398,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>166</v>
       </c>
@@ -3270,7 +3409,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>167</v>
       </c>
@@ -3281,7 +3420,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>168</v>
       </c>
@@ -3292,7 +3431,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>169</v>
       </c>
@@ -3303,7 +3442,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
         <v>170</v>
       </c>
@@ -3412,9 +3551,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>